<commit_message>
minor fix on cross layer
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trinachang/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trinachang/Desktop/TRINA/AU/UNSW/YEAR3/taste of research/birank/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F072AAC-E69C-3A41-AAF8-D63EA32D056C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D8480D-57C2-164F-A58A-C05433581255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{78557671-239F-E04D-A79B-2B60D18E7E4B}"/>
+    <workbookView xWindow="1980" yWindow="1200" windowWidth="28040" windowHeight="17440" xr2:uid="{78557671-239F-E04D-A79B-2B60D18E7E4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="14">
   <si>
     <t>ipad</t>
   </si>
@@ -54,13 +54,28 @@
     <t>grey</t>
   </si>
   <si>
-    <t>Australia(importance 5)</t>
-  </si>
-  <si>
-    <t>NZ(importance 3)</t>
-  </si>
-  <si>
-    <t>USA(importance 4)</t>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>Australia(importance 1)</t>
+  </si>
+  <si>
+    <t>NZ(importance 0.5)</t>
+  </si>
+  <si>
+    <t>USA(importance 0.4)</t>
+  </si>
+  <si>
+    <t>AUS-NZ</t>
+  </si>
+  <si>
+    <t>aus</t>
+  </si>
+  <si>
+    <t>nz</t>
   </si>
 </sst>
 </file>
@@ -96,11 +111,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,23 +431,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A4F36E5-C8C7-4B49-8838-479D9D70CF50}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -441,8 +475,29 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -455,8 +510,26 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="2">
+        <v>2</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -469,8 +542,26 @@
       <c r="D4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -483,16 +574,39 @@
       <c r="D5">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="2">
+        <v>2</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -502,8 +616,23 @@
       <c r="D8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -516,8 +645,23 @@
       <c r="D9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -530,8 +674,23 @@
       <c r="D10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>3</v>
+      </c>
+      <c r="K10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -544,16 +703,31 @@
       <c r="D11">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" s="2">
+        <v>1</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>3</v>
       </c>
@@ -563,8 +737,11 @@
       <c r="D14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -577,8 +754,11 @@
       <c r="D15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -591,8 +771,11 @@
       <c r="D16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -604,6 +787,9 @@
       </c>
       <c r="D17">
         <v>5</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>